<commit_message>
BB 6.14 ActiveJob and Advanced ActionCable
</commit_message>
<xml_diff>
--- a/config/Job_track_spreadsheet.xlsx
+++ b/config/Job_track_spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="17460" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Linkedin" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Indeed.de" sheetId="9" r:id="rId7"/>
     <sheet name="Spontaneous applicant" sheetId="7" r:id="rId8"/>
     <sheet name="CV &amp; profiles" sheetId="10" r:id="rId9"/>
+    <sheet name="talent.io" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="91">
   <si>
     <t>Add reference</t>
   </si>
@@ -77,9 +78,6 @@
     <t>Ruby on Rails Developer</t>
   </si>
   <si>
-    <t>CV sent</t>
-  </si>
-  <si>
     <t>Senior Ruby on Rails Developer</t>
   </si>
   <si>
@@ -105,13 +103,233 @@
   </si>
   <si>
     <t>Frontend Developer</t>
+  </si>
+  <si>
+    <t>Received a call suggesting new openings</t>
+  </si>
+  <si>
+    <t>Talent.io</t>
+  </si>
+  <si>
+    <t>Profile created but Cv info not filled in yet</t>
+  </si>
+  <si>
+    <t>AJAX and Jekyll added</t>
+  </si>
+  <si>
+    <t>Contacted person</t>
+  </si>
+  <si>
+    <t>Babbel</t>
+  </si>
+  <si>
+    <t>Waler Roman</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/walter-roman-45740799</t>
+  </si>
+  <si>
+    <t>emailed trough Github</t>
+  </si>
+  <si>
+    <t>Frontend Engineer</t>
+  </si>
+  <si>
+    <t>Bruno Abrantes</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/brunoabrantes</t>
+  </si>
+  <si>
+    <t>Senior Software Engineer</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/berndnaehler</t>
+  </si>
+  <si>
+    <t>Bernard Nähler</t>
+  </si>
+  <si>
+    <t>Senior Full Stack Developer</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/175472430?refId=b243b9c8-b5c5-45a4-9157-5b68fe83e7fa&amp;trk=jobshomev2_jymbii</t>
+  </si>
+  <si>
+    <t>sent</t>
+  </si>
+  <si>
+    <t>Senior Full Stack Software Engineer</t>
+  </si>
+  <si>
+    <t>Markus Witte</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Babblel</t>
+  </si>
+  <si>
+    <t>approached through facebook</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/markuswi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs2/view/196480428?trk=job_view_similar_jobs</t>
+  </si>
+  <si>
+    <t>Pepper.com - The World's Largest Deal Community</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Frontend Developer - Javascript - Angularjs</t>
+  </si>
+  <si>
+    <t>European recruitment</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs2/view/196403336?trk=job_view_similar_jobs</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs2/view/175479795?trk=job_view_similar_jobs</t>
+  </si>
+  <si>
+    <t>Affinitas (eDarling, EliteSingles)</t>
+  </si>
+  <si>
+    <t>Affinitas</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs2/view/196950213?trk=job_view_similar_jobs</t>
+  </si>
+  <si>
+    <t>Mass-Tech Group</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs2/view/205299048?trk=job_view_similar_jobs</t>
+  </si>
+  <si>
+    <t>Frontend Web Developer (m/f)</t>
+  </si>
+  <si>
+    <t>Freenet digital</t>
+  </si>
+  <si>
+    <t>https://www.smartrecruiters.com/kaufDA/95429937-front-end-developer-online-marketing-f-m-</t>
+  </si>
+  <si>
+    <t>Frontend Developer - Online Marketing (m/f)</t>
+  </si>
+  <si>
+    <t>bonial.com</t>
+  </si>
+  <si>
+    <t>http://de.indeed.com/viewjob?jk=48654845eb74977f&amp;q=web+developer&amp;l=Berlin&amp;tk=1at8iufd1545ea3l&amp;from=web&amp;advn=8637124929343532&amp;sjdu=0f40MzUt-zIomRqQ49ckdOS-NY8tQxyc6HtzrQ86-QpWoulEISD4b28_NIksm7XP9hXaurLHdAD_1nXuLyKUM0YCsogoUgYdtnGUd7qMGOA&amp;pub=4a1b367933fd867b19b072952f68dceb</t>
+  </si>
+  <si>
+    <t>Frontend Developer (m / f) </t>
+  </si>
+  <si>
+    <t>surf GmbH &amp; Co. KG</t>
+  </si>
+  <si>
+    <t>Indeed</t>
+  </si>
+  <si>
+    <t>Profile needs update</t>
+  </si>
+  <si>
+    <t>http://de.indeed.com/cmp/Jonas-und-der-Wolf/jobs/Frontend-Developer-Vollzeit-db2d38b1c7cacf85?sjdu=Aj8fnI-wbineBf11iHvnFvqrOyNp5Ca64GLYvYu5pCkWoSxdO-5VGYBnd5eLs9tPXdjEhLMLuUCqZJvFulXt3yao3O4Ty-25Pd34z-g354uEtjWhjZZ6Zeg_oByEv90I</t>
+  </si>
+  <si>
+    <t>Frontend Developer (m / f) full-time from now on </t>
+  </si>
+  <si>
+    <r>
+      <t>Jonah and the Wolf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>http://de.indeed.com/cmp/Ayuda-GmbH/jobs/Frontend-Web-Developer-d060a772efa67a45?sjdu=Aj8fnI-wbineBf11iHvnFvqrOyNp5Ca64GLYvYu5pClQP0v68BMEAunJDRwWYTa7urHWSjZyQ2GVMhIMpmMpq61I2RZZov26JerQPEcHmFc</t>
+  </si>
+  <si>
+    <t>Frontend Web Developer (m / w) </t>
+  </si>
+  <si>
+    <r>
+      <t>AYUDA MEDIA SYSTEMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>https://campanda.staffboard.de/public/job/424/frontend-developer-m-w</t>
+  </si>
+  <si>
+    <t>CampAnda GMH</t>
+  </si>
+  <si>
+    <t>http://www.aperto.com/de/de/jobs/junior-frontend-developer-move-m-w-berlin0</t>
+  </si>
+  <si>
+    <t>Frontend Developer Junior (m/w)...</t>
+  </si>
+  <si>
+    <t>Aperto</t>
+  </si>
+  <si>
+    <t>http://de.indeed.com/viewjob?jk=48c9ff3d6cbf0ea7&amp;q=web+developer&amp;l=Berlin&amp;tk=1at8iufd1545ea3l&amp;from=web</t>
+  </si>
+  <si>
+    <t>Web Developer HTML/CSS (m/f) </t>
+  </si>
+  <si>
+    <t>Homeday GmbH</t>
+  </si>
+  <si>
+    <t>https://app.jobvite.com/CompanyJobs/Careers.aspx?k=Job&amp;su=fhQ9VfwV&amp;c=qIF9Vfwb&amp;j=oAur2fwh&amp;s=Indeed</t>
+  </si>
+  <si>
+    <t>Auto1</t>
+  </si>
+  <si>
+    <t>HTML5/CSS3 FRONTEND DEVELOPER (M/F)</t>
+  </si>
+  <si>
+    <t>https://modoweb-images-production.s3-eu-west-1.amazonaws.com/job_applications/job_application/document/241/Frontend-EN_Final.pdf?utm_source=Indeed&amp;utm_medium=organic&amp;utm_campaign=Indeed</t>
+  </si>
+  <si>
+    <t>modomoto</t>
+  </si>
+  <si>
+    <t>Frontend Web Developer (f/m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,12 +373,31 @@
       <name val="Inherit"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -204,7 +441,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -216,8 +453,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -227,20 +476,35 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="19"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,18 +834,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="102" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,16 +874,16 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7">
         <v>42633</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -627,22 +891,211 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="7">
         <v>42634</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
+      </c>
+      <c r="C5" s="7">
+        <v>42665</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +1289,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -866,6 +1319,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -876,13 +1330,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -905,6 +1365,166 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -923,17 +1543,21 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -954,18 +1578,109 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="5" spans="1:8" ht="18">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="7">
+        <v>42635</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
       <c r="H5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="H6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -976,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -988,15 +1703,18 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1722,7 @@
         <v>42633</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1012,74 +1730,96 @@
         <v>42633</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5">
+        <v>42634</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42635</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="5">
-        <v>42633</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>42634</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1087,31 +1827,31 @@
         <v>42633</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:3">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="B32" s="5"/>
     </row>
     <row r="33" spans="2:2">

</xml_diff>